<commit_message>
cambio dependencia en sercotec
</commit_message>
<xml_diff>
--- a/Maestros.xlsx
+++ b/Maestros.xlsx
@@ -1107,13 +1107,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>99</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>100</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>101</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>153</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>102</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>103</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>133</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>104</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>158</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>159</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>105</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>162</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>163</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>108</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>110</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>111</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>112</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>113</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>114</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>164</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>165</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>116</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>166</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>136</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>117</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>118</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>167</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>179</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>137</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>16</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>149</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>18</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>20</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>22</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>138</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>23</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>139</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>168</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>180</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>140</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>25</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>150</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>141</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>26</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>142</v>
       </c>
@@ -1602,15 +1602,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>119</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>28</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>120</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>143</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>121</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>122</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>123</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>177</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>124</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>144</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>125</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>151</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>152</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>146</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>126</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>127</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>170</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>171</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>172</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>173</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>174</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>155</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>128</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>147</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>29</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>30</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>31</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>129</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>176</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>32</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>33</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>34</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>35</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>130</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>90</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>72</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>73</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>74</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>178</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>92</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>94</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>95</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>156</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>76</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>96</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>175</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>77</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>78</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>79</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>80</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>81</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>82</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>83</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>84</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>85</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>86</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>88</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>131</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>37</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>38</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>39</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>40</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>41</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>42</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>43</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>44</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>45</v>
       </c>
@@ -2155,7 +2155,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B129"/>
+  <autoFilter ref="A1:B129">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Ministerio de Relaciones Exteriores"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>